<commit_message>
add combobox and realissed full changed data (MP to US)
</commit_message>
<xml_diff>
--- a/Шаблон соревнований.xlsx
+++ b/Шаблон соревнований.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislav/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Projects\Scoreboard_ProfiRu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{718D0792-CDAB-4847-AB6B-2121EFCA5164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="740" windowWidth="28240" windowHeight="16680" xr2:uid="{B6FFDD8E-327E-684C-A410-93EA142F0C20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Спортсмен</t>
   </si>
@@ -74,12 +73,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Таиров Дамир Шамилевич </t>
-  </si>
-  <si>
-    <t>Одинцовская СОШ 3  ПН СР ПТ</t>
-  </si>
-  <si>
     <t>Макаров Егор Андреевич</t>
   </si>
   <si>
@@ -90,13 +83,52 @@
   </si>
   <si>
     <t xml:space="preserve">Ибрагимов Лёми </t>
+  </si>
+  <si>
+    <t>Иванов Иван Иванович</t>
+  </si>
+  <si>
+    <t>Сидоров Петр Сергеевич</t>
+  </si>
+  <si>
+    <t>Соловьев Андрей Петрович</t>
+  </si>
+  <si>
+    <t>Сорокин Алексей Александрович</t>
+  </si>
+  <si>
+    <t>МБОУ СОШ 6</t>
+  </si>
+  <si>
+    <t>Лицей №7</t>
+  </si>
+  <si>
+    <t>Гимназия ДГТУ</t>
+  </si>
+  <si>
+    <t>СОШ №582</t>
+  </si>
+  <si>
+    <t>Антонов Алексей</t>
+  </si>
+  <si>
+    <t>Смелов Егор</t>
+  </si>
+  <si>
+    <t>Шмелев Вячислав</t>
+  </si>
+  <si>
+    <t>Друзь Иван</t>
+  </si>
+  <si>
+    <t>Таиров Дамир</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -462,19 +494,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1740C67-1349-764B-BA39-373F8BA0CFD1}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9" activeCellId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.87890625" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -523,15 +555,15 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>43534</v>
@@ -545,14 +577,122 @@
       <c r="E3">
         <v>28</v>
       </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
       <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
+      <c r="B4" s="1">
+        <v>38384</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>38444</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>38902</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>38058</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>